<commit_message>
Formulaire de modification de dossier
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin3.xlsx
+++ b/FichesTemps/MaximeAubin3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{431BE66C-A63A-488B-BBD7-453802979BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DF8292-9677-46FA-91C8-75E79B45BAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="92">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -421,6 +421,9 @@
   </si>
   <si>
     <t>Formulaire de modification de dossier</t>
+  </si>
+  <si>
+    <t>09/02/2023</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1823,7 @@
   <dimension ref="A1:F466"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,7 +1918,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -2035,10 +2038,16 @@
       <c r="D19" s="52"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
+      <c r="A20" s="48" t="s">
+        <v>91</v>
+      </c>
       <c r="B20" s="52"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="52"/>
+      <c r="C20" s="53">
+        <v>3</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="51"/>

</xml_diff>

<commit_message>
Draft de Documentation client
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin3.xlsx
+++ b/FichesTemps/MaximeAubin3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DF8292-9677-46FA-91C8-75E79B45BAE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA93005-DA0F-4A89-BAE3-C29DA50B42D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="93">
   <si>
     <t>Fiche d'évaluation du travail d'équipe</t>
   </si>
@@ -424,6 +424,9 @@
   </si>
   <si>
     <t>09/02/2023</t>
+  </si>
+  <si>
+    <t>Nettoyage et debug du formulaire de dossier</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1826,7 @@
   <dimension ref="A1:F466"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1918,7 +1921,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>14</v>
+        <v>16.5</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -2043,17 +2046,23 @@
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="53">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" s="52" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
+      <c r="A21" s="48" t="s">
+        <v>91</v>
+      </c>
       <c r="B21" s="52"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="52"/>
+      <c r="C21" s="53">
+        <v>1.5</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="51"/>

</xml_diff>

<commit_message>
Documentation prog et client
</commit_message>
<xml_diff>
--- a/FichesTemps/MaximeAubin3.xlsx
+++ b/FichesTemps/MaximeAubin3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45CBD9E-78C2-41C8-A327-D392AE94C70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEF1E4F-45EF-44B7-B985-360B2F296AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="bsnEa0N1OcI6znPoPEcq3AHEi57LtmD/hoPfLk9LAHbO8ZgF/KxDU64xoRN551lSOgXhKiKNTKiOVsg9sOO7CQ==" workbookSaltValue="Arsw55Oy1Kl5wQ7vU+yWcQ==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="768" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -1838,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B1E992-A4D6-4269-AA92-453ABD10AC9B}">
   <dimension ref="A1:F466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="C9" s="47">
         <f>SUM(C11:C466)</f>
-        <v>22.5</v>
+        <v>24.5</v>
       </c>
       <c r="D9" s="46" t="s">
         <v>64</v>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="B18" s="52"/>
       <c r="C18" s="53">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="D18" s="52" t="s">
         <v>85</v>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="B21" s="52"/>
       <c r="C21" s="53">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D21" s="52" t="s">
         <v>87</v>

</xml_diff>